<commit_message>
Computed region quality metrics and ploted time of L vs L square (L2)
</commit_message>
<xml_diff>
--- a/Benchmarking/Benchmarking.xlsx
+++ b/Benchmarking/Benchmarking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>N</t>
   </si>
@@ -49,10 +49,142 @@
     <t>(s)</t>
   </si>
   <si>
-    <t>&lt;- something weird (L) ??</t>
-  </si>
-  <si>
-    <t>&lt;- something weird (sys L) ??</t>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>GCE</t>
+  </si>
+  <si>
+    <t>VoI</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>Ceramic</t>
+  </si>
+  <si>
+    <t>Grave</t>
+  </si>
+  <si>
+    <t>Llama</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>0.0665</t>
+  </si>
+  <si>
+    <t>0.4662</t>
+  </si>
+  <si>
+    <t>0.9441</t>
+  </si>
+  <si>
+    <t>0.0534</t>
+  </si>
+  <si>
+    <t>0.9817</t>
+  </si>
+  <si>
+    <t>0.0117</t>
+  </si>
+  <si>
+    <t>0.1677</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9796</t>
+  </si>
+  <si>
+    <t>0.0137</t>
+  </si>
+  <si>
+    <t>0.1837</t>
+  </si>
+  <si>
+    <t>0.9840</t>
+  </si>
+  <si>
+    <t>0.0128</t>
+  </si>
+  <si>
+    <t>0.1432</t>
+  </si>
+  <si>
+    <t>0.9820</t>
+  </si>
+  <si>
+    <t>0.0144</t>
+  </si>
+  <si>
+    <t>0.1558</t>
+  </si>
+  <si>
+    <t>0.9747</t>
+  </si>
+  <si>
+    <t>0.0240</t>
+  </si>
+  <si>
+    <t>0.1781</t>
+  </si>
+  <si>
+    <t>0.9729</t>
+  </si>
+  <si>
+    <t>0.0255</t>
+  </si>
+  <si>
+    <t>0.1857</t>
+  </si>
+  <si>
+    <t>0.931</t>
+  </si>
+  <si>
+    <t>0.401</t>
+  </si>
+  <si>
+    <t>0.9868</t>
+  </si>
+  <si>
+    <t>0.0094</t>
+  </si>
+  <si>
+    <t>0.1151</t>
+  </si>
+  <si>
+    <t>0.9864</t>
+  </si>
+  <si>
+    <t>0.0097</t>
+  </si>
+  <si>
+    <t>0.1172</t>
+  </si>
+  <si>
+    <t>0.9900</t>
+  </si>
+  <si>
+    <t>0.0072</t>
+  </si>
+  <si>
+    <t>0.0852</t>
+  </si>
+  <si>
+    <t>0.9899</t>
+  </si>
+  <si>
+    <t>0.0073</t>
+  </si>
+  <si>
+    <t>0.0857</t>
   </si>
 </sst>
 </file>
@@ -130,7 +262,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -146,8 +278,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,9 +306,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -172,7 +319,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="33">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -180,6 +327,15 @@
     <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -187,6 +343,15 @@
     <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -272,8 +437,8 @@
                 <c:pt idx="1">
                   <c:v>1.41144</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0,000,000">
-                  <c:v>1.07666</c:v>
+                <c:pt idx="2">
+                  <c:v>1.11451</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0,000,000">
                   <c:v>0.844891</c:v>
@@ -308,11 +473,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2108987080"/>
-        <c:axId val="-2108894520"/>
+        <c:axId val="-2125779592"/>
+        <c:axId val="-2126158680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2108987080"/>
+        <c:axId val="-2125779592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,7 +487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108894520"/>
+        <c:crossAx val="-2126158680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -330,7 +495,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108894520"/>
+        <c:axId val="-2126158680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,7 +506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108987080"/>
+        <c:crossAx val="-2125779592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -439,13 +604,13 @@
                   <c:v>9.14904</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.35739</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0,000,000">
-                  <c:v>7.51253</c:v>
+                  <c:v>7.88739</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>6.51</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0,000,000">
-                  <c:v>6.88318</c:v>
+                  <c:v>5.45072</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0,000,000">
                   <c:v>3.7382</c:v>
@@ -477,11 +642,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2109613288"/>
-        <c:axId val="-2077861512"/>
+        <c:axId val="-2125490168"/>
+        <c:axId val="-2125506568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109613288"/>
+        <c:axId val="-2125490168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -491,7 +656,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077861512"/>
+        <c:crossAx val="-2125506568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -499,7 +664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077861512"/>
+        <c:axId val="-2125506568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109613288"/>
+        <c:crossAx val="-2125490168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -602,22 +767,22 @@
             <c:numRef>
               <c:f>L_vs_L2!$G$4:$G$12</c:f>
               <c:numCache>
-                <c:formatCode>#.##0000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="0,000,000">
-                  <c:v>96.8308</c:v>
+                <c:pt idx="0">
+                  <c:v>160.218</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.7922</c:v>
+                  <c:v>124.42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.1592</c:v>
+                  <c:v>102.284</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0,000,000">
-                  <c:v>57.2807</c:v>
+                  <c:v>53.2807</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0,000,000">
-                  <c:v>16.014</c:v>
+                  <c:v>18.014</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0,000,000">
                   <c:v>8.54009</c:v>
@@ -646,11 +811,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2130115768"/>
-        <c:axId val="-2078187528"/>
+        <c:axId val="-2125508248"/>
+        <c:axId val="-2125528776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2130115768"/>
+        <c:axId val="-2125508248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2078187528"/>
+        <c:crossAx val="-2125528776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,18 +833,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2078187528"/>
+        <c:axId val="-2125528776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0,000,000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130115768"/>
+        <c:crossAx val="-2125508248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -771,19 +936,19 @@
             <c:numRef>
               <c:f>L_vs_L2!$H$4:$H$12</c:f>
               <c:numCache>
-                <c:formatCode>#.##0000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="0,000,000">
-                  <c:v>546.904</c:v>
+                <c:pt idx="0">
+                  <c:v>826.812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>450.806</c:v>
+                  <c:v>608.165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>417.897</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0,000,000">
-                  <c:v>223.553</c:v>
+                  <c:v>483.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>247.33</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0,000,000">
                   <c:v>85.1525</c:v>
@@ -815,11 +980,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2077883960"/>
-        <c:axId val="-2077882552"/>
+        <c:axId val="-2125553320"/>
+        <c:axId val="-2125550312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2077883960"/>
+        <c:axId val="-2125553320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077882552"/>
+        <c:crossAx val="-2125550312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -837,18 +1002,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077882552"/>
+        <c:axId val="-2125550312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0,000,000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077883960"/>
+        <c:crossAx val="-2125553320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1323,15 +1488,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="5.1640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" s="1" customFormat="1">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1342,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M12"/>
+  <dimension ref="B2:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B12" sqref="B4:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1354,9 +1739,10 @@
     <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:15">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1379,7 +1765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:15">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1402,7 +1788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:15">
       <c r="B4" s="1">
         <f>C4*D4</f>
         <v>874800</v>
@@ -1413,21 +1799,23 @@
       <c r="D4" s="1">
         <v>810</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1.6721900000000001</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>9.1490399999999994</v>
       </c>
-      <c r="G4" s="6">
-        <v>96.830799999999996</v>
-      </c>
-      <c r="H4" s="6">
-        <v>546.904</v>
-      </c>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="2:13">
+      <c r="G4" s="1">
+        <v>160.21799999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>826.81200000000001</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" s="1">
         <f t="shared" ref="B5:B12" si="0">C5*D5</f>
         <v>708588</v>
@@ -1438,24 +1826,27 @@
       <c r="D5" s="1">
         <v>729</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>1.41144</v>
       </c>
-      <c r="F5" s="8">
-        <v>7.3573899999999997</v>
-      </c>
-      <c r="G5" s="8">
-        <v>94.792199999999994</v>
-      </c>
-      <c r="H5" s="8">
-        <v>450.80599999999998</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="2:13">
+      <c r="F5" s="7">
+        <v>7.8873899999999999</v>
+      </c>
+      <c r="G5" s="1">
+        <v>124.42</v>
+      </c>
+      <c r="H5" s="1">
+        <v>608.16499999999996</v>
+      </c>
+      <c r="I5">
+        <f>H5/G5</f>
+        <v>4.8880003214917211</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="2:15">
       <c r="B6" s="1">
         <f t="shared" si="0"/>
         <v>574000</v>
@@ -1466,24 +1857,27 @@
       <c r="D6" s="1">
         <v>656</v>
       </c>
-      <c r="E6" s="6">
-        <v>1.07666</v>
-      </c>
-      <c r="F6" s="6">
-        <v>7.5125299999999999</v>
-      </c>
-      <c r="G6" s="8">
-        <v>88.159199999999998</v>
-      </c>
-      <c r="H6" s="8">
-        <v>417.89699999999999</v>
-      </c>
-      <c r="J6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="2:13">
+      <c r="E6" s="7">
+        <v>1.1145099999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6.51</v>
+      </c>
+      <c r="G6" s="1">
+        <v>102.28400000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <v>483.23</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I11" si="1">H6/G6</f>
+        <v>4.7243948222595904</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="2:15">
       <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>464920</v>
@@ -1494,23 +1888,29 @@
       <c r="D7" s="1">
         <v>590</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.84489099999999995</v>
       </c>
-      <c r="F7" s="6">
-        <v>6.8831800000000003</v>
-      </c>
-      <c r="G7" s="6">
-        <v>57.280700000000003</v>
-      </c>
-      <c r="H7" s="6">
-        <v>223.553</v>
-      </c>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="2:13">
+      <c r="F7" s="5">
+        <v>5.4507199999999996</v>
+      </c>
+      <c r="G7" s="5">
+        <v>53.280700000000003</v>
+      </c>
+      <c r="H7" s="1">
+        <v>247.33</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>4.6420185920980765</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="2:15">
       <c r="B8" s="2">
-        <f t="shared" ref="B8" si="1">C8*D8</f>
+        <f t="shared" ref="B8" si="2">C8*D8</f>
         <v>270000</v>
       </c>
       <c r="C8" s="2">
@@ -1519,21 +1919,25 @@
       <c r="D8" s="2">
         <v>450</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>0.49203599999999997</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>3.7382</v>
       </c>
-      <c r="G8" s="5">
-        <v>16.013999999999999</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="G8" s="4">
+        <v>18.013999999999999</v>
+      </c>
+      <c r="H8" s="4">
         <v>85.152500000000003</v>
       </c>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="2:13">
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>4.7270178749861227</v>
+      </c>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="2:15">
       <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>172800</v>
@@ -1544,21 +1948,25 @@
       <c r="D9" s="1">
         <v>360</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.28849799999999998</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>2.0629200000000001</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>8.5400899999999993</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>43.197200000000002</v>
       </c>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="2:13">
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>5.0581668343073671</v>
+      </c>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="2:15">
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>110592</v>
@@ -1569,21 +1977,25 @@
       <c r="D10" s="1">
         <v>288</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.19130900000000001</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>1.4237200000000001</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>4.8385899999999999</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>24.169599999999999</v>
       </c>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="2:13">
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>4.9951742139755586</v>
+      </c>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="2:15">
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>39790</v>
@@ -1594,21 +2006,25 @@
       <c r="D11" s="1">
         <v>173</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>6.4155000000000004E-2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>0.50184700000000004</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>1.9563200000000001</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>5.0793600000000003</v>
       </c>
-      <c r="M11" s="7"/>
-    </row>
-    <row r="12" spans="2:13">
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>2.5963850494806575</v>
+      </c>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="2:15">
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>10005</v>
@@ -1619,19 +2035,23 @@
       <c r="D12" s="1">
         <v>87</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>1.8369E-2</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>0.118228</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>0.23206199999999999</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>0.92558499999999999</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="I12">
+        <f>H12/G12</f>
+        <v>3.9885246184209393</v>
+      </c>
+      <c r="M12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>